<commit_message>
updated code and results 20201023
</commit_message>
<xml_diff>
--- a/processed_data/Weekly_distribution/Fierz_CT_weekly_share.xlsx
+++ b/processed_data/Weekly_distribution/Fierz_CT_weekly_share.xlsx
@@ -420,13 +420,13 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>353.813</v>
+        <v>70.76300000000001</v>
       </c>
       <c r="E2">
         <v>79.78400000000001</v>
       </c>
       <c r="F2">
-        <v>0.225</v>
+        <v>1.127</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -440,13 +440,13 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>353.813</v>
+        <v>70.76300000000001</v>
       </c>
       <c r="E3">
         <v>71.081</v>
       </c>
       <c r="F3">
-        <v>0.201</v>
+        <v>1.004</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -460,13 +460,13 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>353.813</v>
+        <v>70.76300000000001</v>
       </c>
       <c r="E4">
         <v>95.29000000000001</v>
       </c>
       <c r="F4">
-        <v>0.269</v>
+        <v>1.347</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -480,13 +480,13 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>353.813</v>
+        <v>70.76300000000001</v>
       </c>
       <c r="E5">
         <v>46.057</v>
       </c>
       <c r="F5">
-        <v>0.13</v>
+        <v>0.651</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -500,13 +500,13 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>353.813</v>
+        <v>70.76300000000001</v>
       </c>
       <c r="E6">
         <v>61.601</v>
       </c>
       <c r="F6">
-        <v>0.174</v>
+        <v>0.871</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -520,13 +520,13 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <v>298.707</v>
+        <v>74.67700000000001</v>
       </c>
       <c r="E7">
         <v>86.52800000000001</v>
       </c>
       <c r="F7">
-        <v>0.29</v>
+        <v>1.159</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -540,13 +540,13 @@
         <v>6</v>
       </c>
       <c r="D8">
-        <v>298.707</v>
+        <v>74.67700000000001</v>
       </c>
       <c r="E8">
         <v>67.343</v>
       </c>
       <c r="F8">
-        <v>0.225</v>
+        <v>0.902</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -560,13 +560,13 @@
         <v>7</v>
       </c>
       <c r="D9">
-        <v>298.707</v>
+        <v>74.67700000000001</v>
       </c>
       <c r="E9">
         <v>58.872</v>
       </c>
       <c r="F9">
-        <v>0.197</v>
+        <v>0.788</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -580,13 +580,13 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>298.707</v>
+        <v>74.67700000000001</v>
       </c>
       <c r="E10">
         <v>85.964</v>
       </c>
       <c r="F10">
-        <v>0.288</v>
+        <v>1.151</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -600,13 +600,13 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <v>280.31</v>
+        <v>70.078</v>
       </c>
       <c r="E11">
         <v>94.297</v>
       </c>
       <c r="F11">
-        <v>0.336</v>
+        <v>1.346</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -620,13 +620,13 @@
         <v>11</v>
       </c>
       <c r="D12">
-        <v>280.31</v>
+        <v>70.078</v>
       </c>
       <c r="E12">
         <v>79.364</v>
       </c>
       <c r="F12">
-        <v>0.283</v>
+        <v>1.133</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -640,13 +640,13 @@
         <v>12</v>
       </c>
       <c r="D13">
-        <v>280.31</v>
+        <v>70.078</v>
       </c>
       <c r="E13">
         <v>59.032</v>
       </c>
       <c r="F13">
-        <v>0.211</v>
+        <v>0.842</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -660,13 +660,13 @@
         <v>13</v>
       </c>
       <c r="D14">
-        <v>280.31</v>
+        <v>70.078</v>
       </c>
       <c r="E14">
         <v>47.616</v>
       </c>
       <c r="F14">
-        <v>0.17</v>
+        <v>0.679</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -700,13 +700,13 @@
         <v>25</v>
       </c>
       <c r="D16">
-        <v>69.41200000000001</v>
+        <v>34.706</v>
       </c>
       <c r="E16">
         <v>37.998</v>
       </c>
       <c r="F16">
-        <v>0.547</v>
+        <v>1.095</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -720,13 +720,13 @@
         <v>26</v>
       </c>
       <c r="D17">
-        <v>69.41200000000001</v>
+        <v>34.706</v>
       </c>
       <c r="E17">
         <v>31.414</v>
       </c>
       <c r="F17">
-        <v>0.453</v>
+        <v>0.905</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -740,13 +740,13 @@
         <v>27</v>
       </c>
       <c r="D18">
-        <v>92.01300000000001</v>
+        <v>23.003</v>
       </c>
       <c r="E18">
         <v>25.582</v>
       </c>
       <c r="F18">
-        <v>0.278</v>
+        <v>1.112</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -760,13 +760,13 @@
         <v>28</v>
       </c>
       <c r="D19">
-        <v>92.01300000000001</v>
+        <v>23.003</v>
       </c>
       <c r="E19">
         <v>24.198</v>
       </c>
       <c r="F19">
-        <v>0.263</v>
+        <v>1.052</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -780,13 +780,13 @@
         <v>29</v>
       </c>
       <c r="D20">
-        <v>92.01300000000001</v>
+        <v>23.003</v>
       </c>
       <c r="E20">
         <v>22.795</v>
       </c>
       <c r="F20">
-        <v>0.248</v>
+        <v>0.991</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -800,13 +800,13 @@
         <v>30</v>
       </c>
       <c r="D21">
-        <v>92.01300000000001</v>
+        <v>23.003</v>
       </c>
       <c r="E21">
         <v>19.437</v>
       </c>
       <c r="F21">
-        <v>0.211</v>
+        <v>0.845</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -820,13 +820,13 @@
         <v>31</v>
       </c>
       <c r="D22">
-        <v>66.995</v>
+        <v>16.749</v>
       </c>
       <c r="E22">
         <v>17.454</v>
       </c>
       <c r="F22">
-        <v>0.261</v>
+        <v>1.042</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -840,13 +840,13 @@
         <v>32</v>
       </c>
       <c r="D23">
-        <v>66.995</v>
+        <v>16.749</v>
       </c>
       <c r="E23">
         <v>16.057</v>
       </c>
       <c r="F23">
-        <v>0.24</v>
+        <v>0.959</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -860,13 +860,13 @@
         <v>34</v>
       </c>
       <c r="D24">
-        <v>66.995</v>
+        <v>16.749</v>
       </c>
       <c r="E24">
         <v>17.52</v>
       </c>
       <c r="F24">
-        <v>0.262</v>
+        <v>1.046</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -880,13 +880,13 @@
         <v>35</v>
       </c>
       <c r="D25">
-        <v>66.995</v>
+        <v>16.749</v>
       </c>
       <c r="E25">
         <v>15.963</v>
       </c>
       <c r="F25">
-        <v>0.238</v>
+        <v>0.953</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -900,13 +900,13 @@
         <v>37</v>
       </c>
       <c r="D26">
-        <v>20.978</v>
+        <v>10.489</v>
       </c>
       <c r="E26">
         <v>12.624</v>
       </c>
       <c r="F26">
-        <v>0.602</v>
+        <v>1.204</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -920,13 +920,13 @@
         <v>38</v>
       </c>
       <c r="D27">
-        <v>20.978</v>
+        <v>10.489</v>
       </c>
       <c r="E27">
         <v>8.353999999999999</v>
       </c>
       <c r="F27">
-        <v>0.398</v>
+        <v>0.796</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -940,13 +940,13 @@
         <v>40</v>
       </c>
       <c r="D28">
-        <v>29.556</v>
+        <v>14.778</v>
       </c>
       <c r="E28">
         <v>12.8</v>
       </c>
       <c r="F28">
-        <v>0.433</v>
+        <v>0.866</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -960,13 +960,13 @@
         <v>41</v>
       </c>
       <c r="D29">
-        <v>29.556</v>
+        <v>14.778</v>
       </c>
       <c r="E29">
         <v>16.756</v>
       </c>
       <c r="F29">
-        <v>0.5669999999999999</v>
+        <v>1.134</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1000,13 +1000,13 @@
         <v>49</v>
       </c>
       <c r="D31">
-        <v>358.981</v>
+        <v>89.745</v>
       </c>
       <c r="E31">
         <v>78.254</v>
       </c>
       <c r="F31">
-        <v>0.218</v>
+        <v>0.872</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1020,13 +1020,13 @@
         <v>50</v>
       </c>
       <c r="D32">
-        <v>358.981</v>
+        <v>89.745</v>
       </c>
       <c r="E32">
         <v>113.79</v>
       </c>
       <c r="F32">
-        <v>0.317</v>
+        <v>1.268</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1040,13 +1040,13 @@
         <v>51</v>
       </c>
       <c r="D33">
-        <v>358.981</v>
+        <v>89.745</v>
       </c>
       <c r="E33">
         <v>92.185</v>
       </c>
       <c r="F33">
-        <v>0.257</v>
+        <v>1.027</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1060,13 +1060,13 @@
         <v>52</v>
       </c>
       <c r="D34">
-        <v>358.981</v>
+        <v>89.745</v>
       </c>
       <c r="E34">
         <v>74.752</v>
       </c>
       <c r="F34">
-        <v>0.208</v>
+        <v>0.833</v>
       </c>
     </row>
   </sheetData>

</xml_diff>